<commit_message>
cuando se genera clasificaciónABC emvía el archivo a cada sección
</commit_message>
<xml_diff>
--- a/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_FITOS.xlsx
+++ b/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_FITOS.xlsx
@@ -4806,45 +4806,37 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>3403010001</t>
+          <t>3902080001</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>ABONO CESPED BOLSA</t>
-        </is>
-      </c>
-      <c r="C51" s="3" t="inlineStr">
-        <is>
-          <t>2KG</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>BARRERA INSECTOS 1L</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr"/>
+      <c r="D51" s="3" t="inlineStr"/>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F51" s="4" t="inlineStr">
         <is>
-          <t>ABONO NATURAL</t>
+          <t>ANTI-PLAGAS</t>
         </is>
       </c>
       <c r="G51" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H51" s="4" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I51" s="4" t="n">
-        <v>129.35</v>
+        <v>131.45</v>
       </c>
       <c r="J51" s="4" t="n">
-        <v>49.7</v>
+        <v>51.44</v>
       </c>
       <c r="K51" s="4" t="n">
         <v>0</v>
@@ -4853,16 +4845,16 @@
         <v>0</v>
       </c>
       <c r="M51" s="5" t="n">
-        <v>6.4</v>
+        <v>5.4</v>
       </c>
       <c r="N51" s="5" t="n">
-        <v>19.1</v>
+        <v>16.1</v>
       </c>
       <c r="O51" s="4" t="n">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="P51" s="4" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="4" t="n">
         <v>0</v>
@@ -4880,7 +4872,7 @@
       </c>
       <c r="U51" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -13 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -11 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V51" s="4" t="inlineStr">
@@ -4897,37 +4889,45 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>3902080001</t>
+          <t>3403010001</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>BARRERA INSECTOS 1L</t>
-        </is>
-      </c>
-      <c r="C52" s="3" t="inlineStr"/>
-      <c r="D52" s="3" t="inlineStr"/>
+          <t>ABONO CESPED BOLSA</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>2KG</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E52" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F52" s="4" t="inlineStr">
         <is>
-          <t>ANTI-PLAGAS</t>
+          <t>ABONO NATURAL</t>
         </is>
       </c>
       <c r="G52" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H52" s="4" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I52" s="4" t="n">
-        <v>131.45</v>
+        <v>129.35</v>
       </c>
       <c r="J52" s="4" t="n">
-        <v>51.44</v>
+        <v>49.7</v>
       </c>
       <c r="K52" s="4" t="n">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>0</v>
       </c>
       <c r="M52" s="5" t="n">
-        <v>5.4</v>
+        <v>6.4</v>
       </c>
       <c r="N52" s="5" t="n">
-        <v>16.1</v>
+        <v>19.1</v>
       </c>
       <c r="O52" s="4" t="n">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="P52" s="4" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="Q52" s="4" t="n">
         <v>0</v>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="U52" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -11 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -13 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V52" s="4" t="inlineStr">
@@ -11788,24 +11788,24 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>3501040001</t>
+          <t>3302070001</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>INSECTICIDA PULGONES 10ML</t>
+          <t>ABONO GERANIOS 750GR</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr"/>
       <c r="D37" s="3" t="inlineStr"/>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F37" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G37" s="4" t="n">
@@ -11815,10 +11815,10 @@
         <v>4</v>
       </c>
       <c r="I37" s="4" t="n">
-        <v>47.8</v>
+        <v>35.96</v>
       </c>
       <c r="J37" s="4" t="n">
-        <v>19.58</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="K37" s="4" t="n">
         <v>0</v>
@@ -11836,7 +11836,7 @@
         <v>-4</v>
       </c>
       <c r="P37" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q37" s="4" t="n">
         <v>0</v>
@@ -11871,24 +11871,24 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>3302070001</t>
+          <t>3501040001</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>ABONO GERANIOS 750GR</t>
+          <t>INSECTICIDA PULGONES 10ML</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr"/>
       <c r="D38" s="3" t="inlineStr"/>
       <c r="E38" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G38" s="4" t="n">
@@ -11898,10 +11898,10 @@
         <v>4</v>
       </c>
       <c r="I38" s="4" t="n">
-        <v>35.96</v>
+        <v>47.8</v>
       </c>
       <c r="J38" s="4" t="n">
-        <v>9.800000000000001</v>
+        <v>19.58</v>
       </c>
       <c r="K38" s="4" t="n">
         <v>0</v>
@@ -11919,7 +11919,7 @@
         <v>-4</v>
       </c>
       <c r="P38" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q38" s="4" t="n">
         <v>0</v>
@@ -12203,37 +12203,37 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>3501110005</t>
+          <t>3902010001</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>INSECTICIDA GERANIOS LU 750 ML</t>
+          <t>ECOFIN ATRAYENTE AVISPAS 150ML</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr"/>
       <c r="D42" s="3" t="inlineStr"/>
       <c r="E42" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F42" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ANTI-PLAGAS</t>
         </is>
       </c>
       <c r="G42" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H42" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I42" s="4" t="n">
-        <v>47.8</v>
+        <v>41.65</v>
       </c>
       <c r="J42" s="4" t="n">
-        <v>21.02</v>
+        <v>15.94</v>
       </c>
       <c r="K42" s="4" t="n">
         <v>0</v>
@@ -12242,16 +12242,16 @@
         <v>0</v>
       </c>
       <c r="M42" s="5" t="n">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="N42" s="5" t="n">
-        <v>5.9</v>
+        <v>10.3</v>
       </c>
       <c r="O42" s="4" t="n">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="P42" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q42" s="4" t="n">
         <v>0</v>
@@ -12269,7 +12269,7 @@
       </c>
       <c r="U42" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -7 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V42" s="4" t="inlineStr">
@@ -12286,37 +12286,37 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>3902010001</t>
+          <t>3501110005</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>ECOFIN ATRAYENTE AVISPAS 150ML</t>
+          <t>INSECTICIDA GERANIOS LU 750 ML</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr"/>
       <c r="D43" s="3" t="inlineStr"/>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F43" s="4" t="inlineStr">
         <is>
-          <t>ANTI-PLAGAS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G43" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H43" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I43" s="4" t="n">
-        <v>41.65</v>
+        <v>47.8</v>
       </c>
       <c r="J43" s="4" t="n">
-        <v>15.94</v>
+        <v>21.02</v>
       </c>
       <c r="K43" s="4" t="n">
         <v>0</v>
@@ -12325,16 +12325,16 @@
         <v>0</v>
       </c>
       <c r="M43" s="5" t="n">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="N43" s="5" t="n">
-        <v>10.3</v>
+        <v>5.9</v>
       </c>
       <c r="O43" s="4" t="n">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="P43" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q43" s="4" t="n">
         <v>0</v>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="U43" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -7 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V43" s="4" t="inlineStr">
@@ -16805,12 +16805,12 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>3501100025</t>
+          <t>3502010005</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>MASTI-CORT CICATRIZANTE 250GR</t>
+          <t>COMPO BIO HU AZUFRE 450GR</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr"/>
@@ -16832,10 +16832,10 @@
         <v>2</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>19.93</v>
+        <v>20.98</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>7.43</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="K25" s="4" t="n">
         <v>8.33</v>
@@ -16853,47 +16853,47 @@
         <v>22</v>
       </c>
       <c r="P25" s="4" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="4" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>63.33</v>
+        <v>102.22</v>
       </c>
       <c r="S25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>20</v>
+      </c>
+      <c r="T25" s="8" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
       <c r="U25" s="3" t="inlineStr">
         <is>
-          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 1012 días.</t>
+          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
         <is>
-          <t>Compra 04/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W25" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>3502010005</t>
+          <t>3501100025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO HU AZUFRE 450GR</t>
+          <t>MASTI-CORT CICATRIZANTE 250GR</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr"/>
@@ -16915,10 +16915,10 @@
         <v>2</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>20.98</v>
+        <v>19.93</v>
       </c>
       <c r="J26" s="4" t="n">
-        <v>8.300000000000001</v>
+        <v>7.43</v>
       </c>
       <c r="K26" s="4" t="n">
         <v>8.33</v>
@@ -16936,35 +16936,35 @@
         <v>22</v>
       </c>
       <c r="P26" s="4" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q26" s="4" t="n">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="R26" s="4" t="n">
-        <v>102.22</v>
+        <v>63.33</v>
       </c>
       <c r="S26" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="T26" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>0</v>
+      </c>
+      <c r="T26" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U26" s="3" t="inlineStr">
         <is>
-          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
+          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 1012 días.</t>
         </is>
       </c>
       <c r="V26" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 04/04/2025</t>
         </is>
       </c>
       <c r="W26" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
     </row>
@@ -19975,12 +19975,12 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>3302210021</t>
+          <t>3302210019</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>ABONO FOLIAR TILLANDSIAS 250ML</t>
+          <t>ABONO FOLIAR CACTUS Y PLANTAS CRASAS 250ML</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr"/>
@@ -20008,7 +20008,7 @@
         <v>2.61</v>
       </c>
       <c r="K63" s="4" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
       <c r="L63" s="4" t="n">
         <v>0</v>
@@ -20020,50 +20020,50 @@
         <v>1.5</v>
       </c>
       <c r="O63" s="4" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="P63" s="4" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Q63" s="4" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="R63" s="4" t="n">
-        <v>0</v>
+        <v>102.22</v>
       </c>
       <c r="S63" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T63" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>20</v>
+      </c>
+      <c r="T63" s="8" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
       <c r="U63" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -1 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
+          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
         </is>
       </c>
       <c r="V63" s="4" t="inlineStr">
         <is>
-          <t>Sin stock</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W63" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>15</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>3302210019</t>
+          <t>3302210021</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>ABONO FOLIAR CACTUS Y PLANTAS CRASAS 250ML</t>
+          <t>ABONO FOLIAR TILLANDSIAS 250ML</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr"/>
@@ -20091,7 +20091,7 @@
         <v>2.61</v>
       </c>
       <c r="K64" s="4" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
       <c r="L64" s="4" t="n">
         <v>0</v>
@@ -20103,38 +20103,38 @@
         <v>1.5</v>
       </c>
       <c r="O64" s="4" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="P64" s="4" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="Q64" s="4" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="R64" s="4" t="n">
-        <v>102.22</v>
+        <v>0</v>
       </c>
       <c r="S64" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="T64" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>0</v>
+      </c>
+      <c r="T64" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U64" s="3" t="inlineStr">
         <is>
-          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -1 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
         </is>
       </c>
       <c r="V64" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Sin stock</t>
         </is>
       </c>
       <c r="W64" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
     </row>
@@ -20470,24 +20470,24 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>3302210005</t>
+          <t>3502020004</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>CANABIUM VITACANN BIOESTIMULADOR 250ML</t>
+          <t>COMPO BIO FUNGICIDA STOP 750ML</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
@@ -20506,7 +20506,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>0</v>
@@ -20515,16 +20515,16 @@
         <v>0</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="P2" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="R2" s="4" t="n">
-        <v>36.67</v>
+        <v>4.44</v>
       </c>
       <c r="S2" s="5" t="n">
         <v>0</v>
@@ -20541,7 +20541,7 @@
       </c>
       <c r="V2" s="4" t="inlineStr">
         <is>
-          <t>Compra 28/04/2025</t>
+          <t>Compra 27/05/2025</t>
         </is>
       </c>
       <c r="W2" s="4" t="inlineStr">
@@ -20553,24 +20553,24 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>3701010006</t>
+          <t>3302170002</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>HERBICIDA DUO (FLUROXI + QUIZALOF)</t>
+          <t>ABONO UNIVERSAL 1,5KG</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>HERBICIDAS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G3" s="4" t="n">
@@ -20589,7 +20589,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>0</v>
@@ -20598,7 +20598,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="P3" s="4" t="n">
         <v>92</v>
@@ -20619,7 +20619,7 @@
       </c>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 71.75€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 50.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V3" s="4" t="inlineStr">
@@ -20636,24 +20636,24 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>3501100022</t>
+          <t>3402050002</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>YNJECT GO PALMERAS (NO VENTA)</t>
+          <t>BRILLO PLANTA NATURAL 800ML</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="3" t="inlineStr"/>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONO NATURAL</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
@@ -20672,7 +20672,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>0</v>
@@ -20681,7 +20681,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="4" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="P4" s="4" t="n">
         <v>92</v>
@@ -20702,7 +20702,7 @@
       </c>
       <c r="U4" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 211.68€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 45.88€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V4" s="4" t="inlineStr">
@@ -20719,12 +20719,12 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>3501100021</t>
+          <t>3501100022</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>YNJECT GO PINO (NO VENTA)</t>
+          <t>YNJECT GO PALMERAS (NO VENTA)</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr"/>
@@ -20755,7 +20755,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>0</v>
@@ -20764,7 +20764,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="P5" s="4" t="n">
         <v>92</v>
@@ -20785,7 +20785,7 @@
       </c>
       <c r="U5" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 47.04€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 211.68€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V5" s="4" t="inlineStr">
@@ -20802,24 +20802,24 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>3501010004</t>
+          <t>3302210022</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>TRIPLE ACCION 1000ML AFIDOR</t>
+          <t>COMPO FERTILIZANTE CICLAMENES 250ML</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr"/>
       <c r="D6" s="3" t="inlineStr"/>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G6" s="4" t="n">
@@ -20838,7 +20838,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>0</v>
@@ -20847,19 +20847,19 @@
         <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="P6" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q6" s="4" t="n">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="R6" s="4" t="n">
-        <v>36.67</v>
+        <v>102.22</v>
       </c>
       <c r="S6" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T6" s="9" t="inlineStr">
         <is>
@@ -20868,12 +20868,12 @@
       </c>
       <c r="U6" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 16.38€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
         <is>
-          <t>Compra 28/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W6" s="4" t="inlineStr">
@@ -20885,24 +20885,24 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>3901160000</t>
+          <t>3301040006</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>FIN DESINFECTANTE SUPERFICIES 1L LU</t>
+          <t>COMPO BIO FERTILIZANTE AQUA DEPOT 1L</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" s="3" t="inlineStr"/>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>ANTI-PLAGAS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G7" s="4" t="n">
@@ -20921,7 +20921,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="M7" s="5" t="n">
         <v>0</v>
@@ -20930,19 +20930,19 @@
         <v>0</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="P7" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q7" s="4" t="n">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="R7" s="4" t="n">
-        <v>17.78</v>
+        <v>86.67</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T7" s="9" t="inlineStr">
         <is>
@@ -20951,12 +20951,12 @@
       </c>
       <c r="U7" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 10% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
         <is>
-          <t>Compra 15/05/2025</t>
+          <t>Compra 14/03/2025</t>
         </is>
       </c>
       <c r="W7" s="4" t="inlineStr">
@@ -20968,12 +20968,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>3502020004</t>
+          <t>3501100021</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO FUNGICIDA STOP 750ML</t>
+          <t>YNJECT GO PINO (NO VENTA)</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
@@ -21004,7 +21004,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M8" s="5" t="n">
         <v>0</v>
@@ -21013,19 +21013,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P8" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q8" s="4" t="n">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="R8" s="4" t="n">
-        <v>4.44</v>
+        <v>102.22</v>
       </c>
       <c r="S8" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T8" s="9" t="inlineStr">
         <is>
@@ -21034,12 +21034,12 @@
       </c>
       <c r="U8" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 47.04€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V8" s="4" t="inlineStr">
         <is>
-          <t>Compra 27/05/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W8" s="4" t="inlineStr">
@@ -21051,24 +21051,24 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>3302210016</t>
+          <t>3501100016</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>VIGORIZANTE FOLIAR CACTUS Y CRASAS 250ML</t>
+          <t>YNJECT CONECTOR PALMERA (NO VENTA)</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr"/>
       <c r="D9" s="3" t="inlineStr"/>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G9" s="4" t="n">
@@ -21087,7 +21087,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>0</v>
@@ -21096,19 +21096,19 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="P9" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="R9" s="4" t="n">
-        <v>63.33</v>
+        <v>102.22</v>
       </c>
       <c r="S9" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T9" s="9" t="inlineStr">
         <is>
@@ -21117,12 +21117,12 @@
       </c>
       <c r="U9" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 23.52€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V9" s="4" t="inlineStr">
         <is>
-          <t>Compra 04/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W9" s="4" t="inlineStr">
@@ -21134,12 +21134,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>3501100015</t>
+          <t>3501100026</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>YNJECT CONECTOR PINO (NO VENTA)</t>
+          <t>BIOFLOWER INSECTICIDA NATURAL NEEMEX 500ML</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr"/>
@@ -21170,7 +21170,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0</v>
@@ -21179,19 +21179,19 @@
         <v>0</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="P10" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>102.22</v>
+        <v>17.78</v>
       </c>
       <c r="S10" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T10" s="9" t="inlineStr">
         <is>
@@ -21200,12 +21200,12 @@
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.88€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 15/05/2025</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
@@ -21217,24 +21217,24 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>3402050002</t>
+          <t>3302210005</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>BRILLO PLANTA NATURAL 800ML</t>
+          <t>CANABIUM VITACANN BIOESTIMULADOR 250ML</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr"/>
       <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>ABONO NATURAL</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
@@ -21253,7 +21253,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0</v>
@@ -21262,19 +21262,19 @@
         <v>0</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P11" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q11" s="4" t="n">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="R11" s="4" t="n">
-        <v>102.22</v>
+        <v>36.67</v>
       </c>
       <c r="S11" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T11" s="9" t="inlineStr">
         <is>
@@ -21283,12 +21283,12 @@
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 45.88€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 28/04/2025</t>
         </is>
       </c>
       <c r="W11" s="4" t="inlineStr">
@@ -21300,24 +21300,24 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>3302170002</t>
+          <t>3501100015</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>ABONO UNIVERSAL 1,5KG</t>
+          <t>YNJECT CONECTOR PINO (NO VENTA)</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr"/>
       <c r="D12" s="3" t="inlineStr"/>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G12" s="4" t="n">
@@ -21336,7 +21336,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="M12" s="5" t="n">
         <v>0</v>
@@ -21345,7 +21345,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="4" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P12" s="4" t="n">
         <v>92</v>
@@ -21366,7 +21366,7 @@
       </c>
       <c r="U12" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 50.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.88€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V12" s="4" t="inlineStr">
@@ -21383,24 +21383,24 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>3301040006</t>
+          <t>3501010004</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO FERTILIZANTE AQUA DEPOT 1L</t>
+          <t>TRIPLE ACCION 1000ML AFIDOR</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr"/>
       <c r="D13" s="3" t="inlineStr"/>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G13" s="4" t="n">
@@ -21419,7 +21419,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>0</v>
@@ -21428,19 +21428,19 @@
         <v>0</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="P13" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q13" s="4" t="n">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="R13" s="4" t="n">
-        <v>86.67</v>
+        <v>36.67</v>
       </c>
       <c r="S13" s="5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T13" s="9" t="inlineStr">
         <is>
@@ -21449,12 +21449,12 @@
       </c>
       <c r="U13" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 10% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
         <is>
-          <t>Compra 14/03/2025</t>
+          <t>Compra 28/04/2025</t>
         </is>
       </c>
       <c r="W13" s="4" t="inlineStr">
@@ -21466,12 +21466,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>3301080002</t>
+          <t>3302210008</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>COMPO REVIT ORQUIDEA MONODOSIS 5X30ML</t>
+          <t>FERTILIZANTE ORQUIDEAS 250ML</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
@@ -21549,24 +21549,24 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>3501100016</t>
+          <t>3301080002</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>YNJECT CONECTOR PALMERA (NO VENTA)</t>
+          <t>COMPO REVIT ORQUIDEA MONODOSIS 5X30ML</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr"/>
       <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G15" s="4" t="n">
@@ -21585,7 +21585,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -21594,19 +21594,19 @@
         <v>0</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q15" s="4" t="n">
-        <v>92</v>
+        <v>4</v>
       </c>
       <c r="R15" s="4" t="n">
-        <v>102.22</v>
+        <v>4.44</v>
       </c>
       <c r="S15" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T15" s="9" t="inlineStr">
         <is>
@@ -21615,12 +21615,12 @@
       </c>
       <c r="U15" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 23.52€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V15" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 27/05/2025</t>
         </is>
       </c>
       <c r="W15" s="4" t="inlineStr">
@@ -21632,24 +21632,24 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>3302210008</t>
+          <t>3701010006</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>FERTILIZANTE ORQUIDEAS 250ML</t>
+          <t>HERBICIDA DUO (FLUROXI + QUIZALOF)</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
       <c r="D16" s="3" t="inlineStr"/>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>HERBICIDAS</t>
         </is>
       </c>
       <c r="G16" s="4" t="n">
@@ -21668,7 +21668,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M16" s="5" t="n">
         <v>0</v>
@@ -21677,19 +21677,19 @@
         <v>0</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P16" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q16" s="4" t="n">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="R16" s="4" t="n">
-        <v>4.44</v>
+        <v>102.22</v>
       </c>
       <c r="S16" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T16" s="9" t="inlineStr">
         <is>
@@ -21698,12 +21698,12 @@
       </c>
       <c r="U16" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 71.75€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V16" s="4" t="inlineStr">
         <is>
-          <t>Compra 27/05/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W16" s="4" t="inlineStr">
@@ -21715,24 +21715,24 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>3501100026</t>
+          <t>3901160000</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BIOFLOWER INSECTICIDA NATURAL NEEMEX 500ML</t>
+          <t>FIN DESINFECTANTE SUPERFICIES 1L LU</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr"/>
       <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ANTI-PLAGAS</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
@@ -21798,12 +21798,12 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>3302210022</t>
+          <t>3302210016</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>COMPO FERTILIZANTE CICLAMENES 250ML</t>
+          <t>VIGORIZANTE FOLIAR CACTUS Y CRASAS 250ML</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr"/>
@@ -21834,7 +21834,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>0</v>
@@ -21843,19 +21843,19 @@
         <v>0</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P18" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q18" s="4" t="n">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="R18" s="4" t="n">
-        <v>102.22</v>
+        <v>63.33</v>
       </c>
       <c r="S18" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T18" s="9" t="inlineStr">
         <is>
@@ -21864,12 +21864,12 @@
       </c>
       <c r="U18" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 16.38€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V18" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 04/04/2025</t>
         </is>
       </c>
       <c r="W18" s="4" t="inlineStr">

</xml_diff>